<commit_message>
Enhance MQTT and SD card command handling
Improved MQTT connection logic with retry attempts and better diagnostics. Status publishing now sends a single JSON string instead of multiple individual messages. Added support for running SD card programs via MQTT commands, including new SD file parsing logic. Updated related buffer handling and diagnostics for SD card operations.
</commit_message>
<xml_diff>
--- a/PinionMotion_MQTT/MQTT_Topics.xlsx
+++ b/PinionMotion_MQTT/MQTT_Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milli079\Documents\GitHub\pinion\PinionMotion_MQTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68524D1-42EC-47B9-94E8-E8EBBEA41A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02560B00-F311-49AA-833C-ECF3F6B466E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="660" windowWidth="24240" windowHeight="13020" xr2:uid="{D689E048-E17F-42C5-8882-2DC925F49AF9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Topic</t>
   </si>
@@ -183,13 +183,22 @@
   </si>
   <si>
     <t>EndProgram</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>(In a JSON array)</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +228,14 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -263,13 +280,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,23 +624,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4621AA26-A173-4EFA-AE7D-655FB9071500}">
-  <dimension ref="A2:J29"/>
+  <dimension ref="A2:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,223 +651,233 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="2"/>
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="3"/>
+      <c r="I3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
       <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" t="s">
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="I6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="6" t="s">
+      <c r="J7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" t="s">
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="8"/>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7" t="s">
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="7" t="s">
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="7" t="s">
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="7" t="s">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="7" t="s">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D29" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="7" t="s">
+    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D30" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add MQTT summary PDF and reorganize UI modules
Added MQTT_Summary.pdf and updated MQTT_Topics.xlsx. Refactored Pinion_Demo_UI by moving MQTT and Serial_Coms related files into dedicated subdirectories, including code, configuration, and assets. Added new Python modules for MQTT and Serial communication, and updated Arduino source files for TeknicZeta.
</commit_message>
<xml_diff>
--- a/PinionMotion_MQTT/MQTT_Topics.xlsx
+++ b/PinionMotion_MQTT/MQTT_Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milli079\Documents\GitHub\pinion\PinionMotion_MQTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02560B00-F311-49AA-833C-ECF3F6B466E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A41D00B-A0A2-43E0-9592-A3AEA65D5E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="660" windowWidth="24240" windowHeight="13020" xr2:uid="{D689E048-E17F-42C5-8882-2DC925F49AF9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Topic</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Alerts</t>
+  </si>
+  <si>
+    <t>As JSON</t>
   </si>
 </sst>
 </file>
@@ -238,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +269,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -276,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -290,12 +302,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -624,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4621AA26-A173-4EFA-AE7D-655FB9071500}">
-  <dimension ref="A2:K30"/>
+  <dimension ref="A2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +660,7 @@
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +677,7 @@
         <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -669,8 +688,14 @@
       <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -680,14 +705,20 @@
       <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="I3" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -697,8 +728,11 @@
       <c r="J4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" t="s">
         <v>49</v>
@@ -713,7 +747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="D6" t="s">
         <v>5</v>
@@ -722,7 +756,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="D7" t="s">
         <v>6</v>
@@ -731,7 +765,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="D8" t="s">
         <v>9</v>
@@ -740,7 +774,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="D9" t="s">
         <v>10</v>
@@ -749,7 +783,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="D10" t="s">
         <v>12</v>
@@ -758,7 +792,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="D11" t="s">
         <v>14</v>
@@ -767,7 +801,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>16</v>
       </c>
@@ -775,7 +809,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>17</v>
       </c>
@@ -783,7 +817,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>18</v>
       </c>
@@ -791,7 +825,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -799,7 +833,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>25</v>
       </c>

</xml_diff>